<commit_message>
Wrote half of the document
</commit_message>
<xml_diff>
--- a/data_schema.xlsx
+++ b/data_schema.xlsx
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t>questionID</t>
   </si>
@@ -72,9 +66,6 @@
     <t>nth_e_or_q</t>
   </si>
   <si>
-    <t>The exam or quiz count number</t>
-  </si>
-  <si>
     <t>weekday</t>
   </si>
   <si>
@@ -99,12 +90,6 @@
     <t>cat3</t>
   </si>
   <si>
-    <t>Major section category</t>
-  </si>
-  <si>
-    <t>Minor Section Category</t>
-  </si>
-  <si>
     <t>approx_time_remaining</t>
   </si>
   <si>
@@ -117,9 +102,6 @@
     <t>course</t>
   </si>
   <si>
-    <t>eith P, FM, or MFE</t>
-  </si>
-  <si>
     <t>creation_hr</t>
   </si>
   <si>
@@ -135,9 +117,6 @@
     <t>nth_exam</t>
   </si>
   <si>
-    <t>the exam count number</t>
-  </si>
-  <si>
     <t>minutes_used</t>
   </si>
   <si>
@@ -163,6 +142,108 @@
   </si>
   <si>
     <t>Hours since the most recent exam</t>
+  </si>
+  <si>
+    <t>hist_subcat_n</t>
+  </si>
+  <si>
+    <t>The number of historical questions in the current question category</t>
+  </si>
+  <si>
+    <t>hist_subcat_diff</t>
+  </si>
+  <si>
+    <t>The sum of difficuly for historical question in the current question subcategory</t>
+  </si>
+  <si>
+    <t>hist_subcat_diff_correct</t>
+  </si>
+  <si>
+    <t>Subset of hist_subcat_diff which were answered correctly</t>
+  </si>
+  <si>
+    <t>The historical sum of minutes_used for correct questions in the current subcategory for exams</t>
+  </si>
+  <si>
+    <t>hist_total_time_e</t>
+  </si>
+  <si>
+    <t>hist_total_time_e_correct</t>
+  </si>
+  <si>
+    <t>The subset of hist_total_time_e which were correct</t>
+  </si>
+  <si>
+    <t>hist_total_time_q</t>
+  </si>
+  <si>
+    <t>Historical total quiz time for questions in current subcategory</t>
+  </si>
+  <si>
+    <t>hist_total_time_q but for exams</t>
+  </si>
+  <si>
+    <t>hist_greater_diff_time_correct</t>
+  </si>
+  <si>
+    <t>hist_greater_diff_time</t>
+  </si>
+  <si>
+    <t>hist_greater_diff_time which were correct</t>
+  </si>
+  <si>
+    <t>Total time spent on exams in current subcategory which have greater difficulty</t>
+  </si>
+  <si>
+    <t>hist_greater_diff</t>
+  </si>
+  <si>
+    <t>same as hist_greater_diff_time but summing over difficulty</t>
+  </si>
+  <si>
+    <t>hist_net_diff</t>
+  </si>
+  <si>
+    <t>same as hist_greater_diff but adds for correct questions and subtracts difficulty for incorrect</t>
+  </si>
+  <si>
+    <t>hist_n_marked</t>
+  </si>
+  <si>
+    <t>Number of marked questions for exams in the current subcategory</t>
+  </si>
+  <si>
+    <t>hist_n_marked_incorrect</t>
+  </si>
+  <si>
+    <t>hist_repeat_question</t>
+  </si>
+  <si>
+    <t>Same as hist_n_marked but only for incorrect questions</t>
+  </si>
+  <si>
+    <t>The total number of times that the current question has already been seen in exams or quizzes</t>
+  </si>
+  <si>
+    <t>Either P, FM, or MFE</t>
+  </si>
+  <si>
+    <t>Exam count number</t>
+  </si>
+  <si>
+    <t>Exam or quiz count number</t>
+  </si>
+  <si>
+    <t>Feature Name</t>
+  </si>
+  <si>
+    <t>Feature Description</t>
+  </si>
+  <si>
+    <t>Major section category, limited to the most frequent 10.  All else are "other"</t>
+  </si>
+  <si>
+    <t>Minor section category, limited to the most frequent 10.  All else are "other"</t>
   </si>
 </sst>
 </file>
@@ -489,223 +570,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
         <v>46</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>